<commit_message>
Fixed the AI's positioning through the rallies Added the ball going to a location based on the quality of the pass/dig
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63507438-8016-40FB-ACD8-B5E050F7D274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BD576-2FDB-4075-A7FA-37D8FB572A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D10"/>
+  <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,24 +474,24 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -513,6 +513,11 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added functionality to send the ball to whichever player was set for both AI and Player
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BD576-2FDB-4075-A7FA-37D8FB572A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53739A66-0727-443E-BFC7-B0CB0D433091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Features to be added</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D11"/>
+  <dimension ref="B3:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="B8:D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,14 +441,14 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -493,31 +493,34 @@
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Quality of life changes - setting player pawns positions during certain phases to make adjusting their positions easier Updated the features list with some things I'm hoping to get some support on
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53739A66-0727-443E-BFC7-B0CB0D433091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35347A55-29E1-4C02-AD64-A42D4E08D3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Features to be added</t>
   </si>
@@ -82,6 +82,25 @@
   </si>
   <si>
     <t>When a set choice is made by either player or AI, send the ball to the location of that player, and not just a tile on the grid</t>
+  </si>
+  <si>
+    <t>BUG - Some squares full</t>
+  </si>
+  <si>
+    <t>Something happens during the rally and the player can't move their pieces to certain tiles</t>
+  </si>
+  <si>
+    <t>Functionality for determining closest player to a ball grid position</t>
+  </si>
+  <si>
+    <t>A function Garrett can use somewhere that returns the closest pawn to a grid position. Going to be used to see who is the closest player to the ball's position and use their passing skill for passing/digging
+also going to use for determining the pass quality -&gt; farther the ball is from a player, the harder it is to pass/dig</t>
+  </si>
+  <si>
+    <t>Turn off setters movement only during certain phases</t>
+  </si>
+  <si>
+    <t>There are certain rally phases where I'd like to set the setters position based on the ball position and not let the player move the setter from there at all</t>
   </si>
 </sst>
 </file>
@@ -133,10 +152,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D15"/>
+  <dimension ref="B3:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +525,17 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>4</v>
@@ -520,6 +556,28 @@
       </c>
       <c r="D15" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Serve now will change location slightly if the serve number is low, possible to serve out of bounds
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35347A55-29E1-4C02-AD64-A42D4E08D3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F6C9FD-3A5D-4CB0-AB08-B3DA448F825B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Features to be added</t>
   </si>
@@ -101,6 +101,24 @@
   </si>
   <si>
     <t>There are certain rally phases where I'd like to set the setters position based on the ball position and not let the player move the setter from there at all</t>
+  </si>
+  <si>
+    <t>Ball serve location based on serve quality</t>
+  </si>
+  <si>
+    <t>When the player or AI serves the ball, if the quality is low the ball position can be changed randomly</t>
+  </si>
+  <si>
+    <t>AI chooses where to attack</t>
+  </si>
+  <si>
+    <t>Have the AI choose randomly where to attack, to be improved in future</t>
+  </si>
+  <si>
+    <t>Ball attack location change based on quality</t>
+  </si>
+  <si>
+    <t>The location of the ball can change randomly based on the quality of the attack, if the attack randomly goes off the grid, it is an error. Need to also reduce the chances for hitting errors to account for these new error chances</t>
   </si>
 </sst>
 </file>
@@ -152,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -162,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,19 +461,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D17"/>
+  <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -476,7 +495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -487,7 +506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -498,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -509,7 +528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -520,63 +539,91 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+    <row r="22" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C23" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D23" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AI now randomly selects a location to attack Player and AI attacks now change location slightly based on attack quality Player and AI can now attack out of bounds, but only determined after the block calculation Reduced the incidents of attacking errors into the net to account for the new error chance
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F6C9FD-3A5D-4CB0-AB08-B3DA448F825B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A8F94-218E-4BF0-928D-15DCA5240AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -180,7 +180,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,24 +550,24 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Passes and digs use the closest players skill level for calculating numbers Player setter now should move into position on digs and passes Updated features list
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A8F94-218E-4BF0-928D-15DCA5240AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D69EA4-4CDC-4680-B5CC-BD184B2D51C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Features to be added</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Limit movement during player blocker reaction phase</t>
-  </si>
-  <si>
-    <t>during the player blocker reaction phase only the blockers should be able to move, and their movement limited to one square from their starting location</t>
-  </si>
-  <si>
     <t>AI serve location determined</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Functionality for determining how many blocks in the area</t>
   </si>
   <si>
-    <t>When a pawn is attacking, determine how many opponents blocks are in a valid area to add to the block quality value of the simulation</t>
-  </si>
-  <si>
     <t>The ball position on the map is placed in one of three locations based on the quality of the pass (1, 2 and 3 passes) for both player and AI</t>
   </si>
   <si>
@@ -90,13 +81,6 @@
     <t>Something happens during the rally and the player can't move their pieces to certain tiles</t>
   </si>
   <si>
-    <t>Functionality for determining closest player to a ball grid position</t>
-  </si>
-  <si>
-    <t>A function Garrett can use somewhere that returns the closest pawn to a grid position. Going to be used to see who is the closest player to the ball's position and use their passing skill for passing/digging
-also going to use for determining the pass quality -&gt; farther the ball is from a player, the harder it is to pass/dig</t>
-  </si>
-  <si>
     <t>Turn off setters movement only during certain phases</t>
   </si>
   <si>
@@ -119,6 +103,40 @@
   </si>
   <si>
     <t>The location of the ball can change randomly based on the quality of the attack, if the attack randomly goes off the grid, it is an error. Need to also reduce the chances for hitting errors to account for these new error chances</t>
+  </si>
+  <si>
+    <t>When a pawn is attacking, determine how many opponents blocks are in a valid area to add to the block quality value of the simulation
+would also be fantastic to take into consideration where the ball is headed when calculating which blocks are close enough to be a factor</t>
+  </si>
+  <si>
+    <t>Function for finding closest player to the ball on attacks and defence</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Edge Case: setter makes a dig, someone else needs to set</t>
+  </si>
+  <si>
+    <t>Use the distance away from the ball to effect the ability to make a dig or pass</t>
+  </si>
+  <si>
+    <t>during the player blocker reaction phase all should be able to move, and their movement limited to one square from their starting location</t>
+  </si>
+  <si>
+    <t>Limit movement during player blocker/defender reaction phase</t>
+  </si>
+  <si>
+    <t>The farther a player is away from the ball, the less likely they are to make a dig. Going to try to have it feel lik 50% is player skill and 50% is proximity to the ball
+equal chance to dig a hard hit right at the target as digging an average hit 3-4 squares away
+Need to consider that the y axis might logically have a greater impact than the x axis to accound for forearm and overhandhand digs
+maybe a system where one tile in the y axis adds 1 difficulty and one tile in the x axis adds 1/2 difficulty</t>
+  </si>
+  <si>
+    <t>BUG -AI not always going to the correct locations off digs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix it </t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,6 +197,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,12 +488,12 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="62.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
@@ -485,145 +510,177 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
+    </row>
+    <row r="14" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D21" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where players can sometimes not move to some tiles - Added logic to update status of tile when player tokens focebly moved in PawnManager.cs
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\NewVBallSim\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D69EA4-4CDC-4680-B5CC-BD184B2D51C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B558478F-28A2-4225-A8AC-8E166EFCB686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2145" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,16 +488,16 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -519,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -530,7 +530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,7 +541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -552,7 +552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -574,7 +574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
@@ -585,7 +585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
@@ -596,7 +596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -607,12 +607,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
@@ -623,7 +623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
@@ -634,18 +634,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -656,7 +656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -667,12 +667,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Added a modifier to the passing calculation that takes into account how far away the passing player is from the ball
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\NewVBallSim\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B558478F-28A2-4225-A8AC-8E166EFCB686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C87D26-60B4-4D45-BB9B-21B8FC0C1D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2145" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,23 +127,43 @@
     <t>Limit movement during player blocker/defender reaction phase</t>
   </si>
   <si>
-    <t>The farther a player is away from the ball, the less likely they are to make a dig. Going to try to have it feel lik 50% is player skill and 50% is proximity to the ball
+    <t>BUG -AI not always going to the correct locations off digs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix it </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The farther a player is away from the ball, the less likely they are to make a dig. Going to try to have it feel lik 50% is player skill and 50% is proximity to the ball
 equal chance to dig a hard hit right at the target as digging an average hit 3-4 squares away
 Need to consider that the y axis might logically have a greater impact than the x axis to accound for forearm and overhandhand digs
-maybe a system where one tile in the y axis adds 1 difficulty and one tile in the x axis adds 1/2 difficulty</t>
-  </si>
-  <si>
-    <t>BUG -AI not always going to the correct locations off digs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix it </t>
+maybe a system where one tile in the y axis adds 1 difficulty and one tile in the x axis adds 1/2 difficulty
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Added distance for passing system, can add something almost exactly the same for digging, with likely a higher mod, making it harder to dig than to pass (but still need to then lower digging thresholds)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +182,13 @@
     <font>
       <strike/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -488,7 +515,7 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
@@ -620,18 +647,18 @@
         <v>5</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added two new features: - distance from the ball now effects the quality and chance of the dig - accurately calculating the number of blockers in the attackers area
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C87D26-60B4-4D45-BB9B-21B8FC0C1D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C889A2A-705F-46E5-B95D-6766A4AEE253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,6 +135,7 @@
   <si>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -149,6 +150,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -188,6 +190,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -225,11 +228,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -515,7 +515,7 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,30 +635,41 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -681,17 +692,6 @@
       </c>
       <c r="D20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated our feature list with the upcoming tasks
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C889A2A-705F-46E5-B95D-6766A4AEE253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1796099F-BD38-4F70-8D7E-70C207B0095E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Features to be added</t>
   </si>
@@ -39,133 +39,63 @@
     <t>Details</t>
   </si>
   <si>
-    <t>AI serve location determined</t>
-  </si>
-  <si>
     <t>Garrett</t>
   </si>
   <si>
-    <t>AI serve location displayed by the ball's position</t>
-  </si>
-  <si>
-    <t>The ai randomly determines a serve location on the court</t>
-  </si>
-  <si>
-    <t>The AI's serve location is displayed by the ball position on the court map</t>
-  </si>
-  <si>
-    <t>Pass/Dig ball position based on quality</t>
-  </si>
-  <si>
-    <t>AI will move into defensive positions</t>
-  </si>
-  <si>
-    <t>At each stage of the rally, the ai will move into appropriate positions on the court</t>
-  </si>
-  <si>
-    <t>Functionality for determining how many blocks in the area</t>
-  </si>
-  <si>
-    <t>The ball position on the map is placed in one of three locations based on the quality of the pass (1, 2 and 3 passes) for both player and AI</t>
-  </si>
-  <si>
-    <t>When the set choice is made, ball is sent to the players location</t>
-  </si>
-  <si>
-    <t>When a set choice is made by either player or AI, send the ball to the location of that player, and not just a tile on the grid</t>
-  </si>
-  <si>
-    <t>BUG - Some squares full</t>
-  </si>
-  <si>
-    <t>Something happens during the rally and the player can't move their pieces to certain tiles</t>
-  </si>
-  <si>
-    <t>Turn off setters movement only during certain phases</t>
-  </si>
-  <si>
-    <t>There are certain rally phases where I'd like to set the setters position based on the ball position and not let the player move the setter from there at all</t>
-  </si>
-  <si>
-    <t>Ball serve location based on serve quality</t>
-  </si>
-  <si>
-    <t>When the player or AI serves the ball, if the quality is low the ball position can be changed randomly</t>
-  </si>
-  <si>
-    <t>AI chooses where to attack</t>
-  </si>
-  <si>
-    <t>Have the AI choose randomly where to attack, to be improved in future</t>
-  </si>
-  <si>
-    <t>Ball attack location change based on quality</t>
-  </si>
-  <si>
-    <t>The location of the ball can change randomly based on the quality of the attack, if the attack randomly goes off the grid, it is an error. Need to also reduce the chances for hitting errors to account for these new error chances</t>
-  </si>
-  <si>
-    <t>When a pawn is attacking, determine how many opponents blocks are in a valid area to add to the block quality value of the simulation
-would also be fantastic to take into consideration where the ball is headed when calculating which blocks are close enough to be a factor</t>
-  </si>
-  <si>
-    <t>Function for finding closest player to the ball on attacks and defence</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Edge Case: setter makes a dig, someone else needs to set</t>
-  </si>
-  <si>
-    <t>Use the distance away from the ball to effect the ability to make a dig or pass</t>
-  </si>
-  <si>
-    <t>during the player blocker reaction phase all should be able to move, and their movement limited to one square from their starting location</t>
-  </si>
-  <si>
-    <t>Limit movement during player blocker/defender reaction phase</t>
-  </si>
-  <si>
-    <t>BUG -AI not always going to the correct locations off digs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix it </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The farther a player is away from the ball, the less likely they are to make a dig. Going to try to have it feel lik 50% is player skill and 50% is proximity to the ball
-equal chance to dig a hard hit right at the target as digging an average hit 3-4 squares away
-Need to consider that the y axis might logically have a greater impact than the x axis to accound for forearm and overhandhand digs
-maybe a system where one tile in the y axis adds 1 difficulty and one tile in the x axis adds 1/2 difficulty
+    <t>AI will react to player pawns positions</t>
+  </si>
+  <si>
+    <t>Gamify this thing</t>
+  </si>
+  <si>
+    <t>This thing is a prototype currently, lets move to make it more gamified
+       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here</t>
+  </si>
+  <si>
+    <t>Balance this thang</t>
+  </si>
+  <si>
+    <t>Game is quite unbalanced currently, take another look at each interaction and adjust the numbers so the results make more sense
+Examples: 
+tools more likely when the attacker hitting at only one hand, rather than two.
+Players make more digs when the ball is near them, and less digs when the ball is farther away
+back row players are less likely to score than front row players, but also less likely to get blocked</t>
+  </si>
+  <si>
+    <t>Add some sounds you idiot</t>
+  </si>
+  <si>
+    <t>Add some basic sound manager functionality into the game
+ball contacts, blocks, hits ball hitting the ground, success sound, fail sound etc.
+announcer lines to take place of the debug text currently being printed, with several variations for each
+some light music for menus and gameplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
+ First step here is to get the AI blockers to move into a better position to defend agains the player
+ There are 3 AI blockers at any time and they are in positions 2, 3 and 4 
+ I have the RotationManager script tracking each pawns position (RotationManager.aiPositionsArray[2], aiPositionsArray[3] and aiPositionsArray[4] are the AI blockers
+STEP 1: A function that will have the AI blockers move one (or x) square(s) closer to where the player has set the ball
+ this function will be called in the RallyManagerV2 script after the player makes their set choice, but before the player decides where they want to attack the ball
+STEP 2: adding on to step 1, if a blocker is &gt;3 squares away from the ball in the y axis, they will move one square towards the ball and one square away from the net
+STEP 3: Some functionality for setting the AI blockers position based on their "matchup" on the other side
+ AI blockers will position themselves directly across from their matchup, the matchups are as follows:
+aiPositionsArray[2] matches up with playerPositionsArray[4]
+aiPositionsArray[3] matches up with playerPositionsArray[3]
+aiPositionsArray[4] matches up with playerPositionsArray[2], basically the match ups are who would be standing across the net from each other in the front row
+ if one of the match ups is a setter, that player should line up in front of a different front row player, sharing a match up with one of their fellow blockers. So this means when the player setter is in the front row, there will always be 2 ai lined up on one front row playerpawn and 1 ai lined up on the other front row playerpawn
+TDLR
+Step 1: AI blockers move towards the ball to try and block it once the player has made a set
+Step 2: AI blocker that is not close enough to block, steps away from the net and becomes an additional defender
+Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
 </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Added distance for passing system, can add something almost exactly the same for digging, with likely a higher mod, making it harder to dig than to pass (but still need to then lower digging thresholds)</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,22 +106,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -221,16 +135,18 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D23"/>
+  <dimension ref="B3:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,180 +451,229 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some minor bugs, lowered the wait times between phases for faster playing, updated the features list with some bugs and next features
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1796099F-BD38-4F70-8D7E-70C207B0095E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4E81E8-16E6-45DF-A89E-EABFC7A0FB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Features to be added</t>
   </si>
@@ -90,12 +90,75 @@
 Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
 </t>
   </si>
+  <si>
+    <t>Debug this bitch</t>
+  </si>
+  <si>
+    <t>when the setter makes a dig, have someone else come in and set the ball</t>
+  </si>
+  <si>
+    <t>Setter updates</t>
+  </si>
+  <si>
+    <t>Serve Receive Rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
+Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
+need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>player transition to offensive positions, players jump into place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">player transitioning to defensive positions happens after ai transitions to offence, should be same time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>player setter can still be moved around during offensive phase
+when calculating the closest pawn, use the updated location and not the indicators location
+stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +170,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -147,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,17 +514,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="64" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -462,7 +546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -473,18 +557,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -495,182 +579,200 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Fixed a bug where setter could still be moved during offensive set up phase
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4E81E8-16E6-45DF-A89E-EABFC7A0FB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF234537-F812-4BF2-983D-E3585F775AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,6 +138,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">player transitioning to defensive positions happens after ai transitions to offence, should be same time
+player setter can still be moved around during offensive phase
 </t>
     </r>
     <r>
@@ -148,8 +149,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>player setter can still be moved around during offensive phase
-when calculating the closest pawn, use the updated location and not the indicators location
+      <t>when calculating the closest pawn, use the updated location and not the indicators location
 stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location</t>
     </r>
   </si>

</xml_diff>

<commit_message>
Fixed a bug where the closest player was being calculated base on the ball indicator rather than its updated location also uncovered and fixed an issue where the block was also being calculated in the same way, updated so that the raycast heads towards the updated location rather than the original set location
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF234537-F812-4BF2-983D-E3585F775AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66197D96-9D80-443F-A838-9ED0541ED996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,6 +139,7 @@
       </rPr>
       <t xml:space="preserve">player transitioning to defensive positions happens after ai transitions to offence, should be same time
 player setter can still be moved around during offensive phase
+when calculating the closest pawn, use the updated location and not the indicators location
 </t>
     </r>
     <r>
@@ -149,8 +150,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>when calculating the closest pawn, use the updated location and not the indicators location
-stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location</t>
+      <t>stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location</t>
     </r>
   </si>
 </sst>

</xml_diff>

<commit_message>
Added functionality to handle when the setter makes a dig, now right side player will come in and set Finally fixed a damn bug where the ball would sometimes not update properly (coroutine was still trying to lerp the ball but not reaching exact location sometimes) Also FInally fixed a damn bug where tiles would be occupied randomly (I was moving digging/passing players towards the ball to make a dig without freeing up the tile they were moving from)
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66197D96-9D80-443F-A838-9ED0541ED996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46F4B91-0ACB-4E9D-B8A4-8966311D42BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,20 +137,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">player transitioning to defensive positions happens after ai transitions to offence, should be same time
+      <t>player transitioning to defensive positions happens after ai transitions to offence, should be same time
 player setter can still be moved around during offensive phase
 when calculating the closest pawn, use the updated location and not the indicators location
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location</t>
+stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location (Maybe Fixed) Finally fixed this thing (was moving the digging/passing player towards the ball without releasing their tile)</t>
     </r>
   </si>
 </sst>
@@ -210,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,6 +220,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -514,17 +510,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="345" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -546,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -557,7 +553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -568,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -579,7 +575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
@@ -590,18 +586,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
@@ -612,167 +608,167 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Added basic functionality to keep players pawns in rotation when setting up on serve recieve
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46F4B91-0ACB-4E9D-B8A4-8966311D42BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EDBB41-08FD-4C63-BBE0-7BF7CD128922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,11 +101,6 @@
   </si>
   <si>
     <t>Serve Receive Rotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
-Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
-need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
   </si>
   <si>
     <r>
@@ -141,6 +136,30 @@
 player setter can still be moved around during offensive phase
 when calculating the closest pawn, use the updated location and not the indicators location
 stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location (Maybe Fixed) Finally fixed this thing (was moving the digging/passing player towards the ball without releasing their tile)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
+Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
     </r>
   </si>
 </sst>
@@ -583,7 +602,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -605,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added functionality for AI blockers to react and move towards the ball, still some kinks to be worked out but is mostly working
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EDBB41-08FD-4C63-BBE0-7BF7CD128922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0AD52F-B3D2-402F-A308-E87D45C225CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,17 +550,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="345" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -627,10 +616,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+    <row r="11" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>

</xml_diff>

<commit_message>
pushing some updates to the features list document
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0AD52F-B3D2-402F-A308-E87D45C225CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF39F274-3DCA-4B75-A89C-1B9802356102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,10 +48,6 @@
     <t>Gamify this thing</t>
   </si>
   <si>
-    <t>This thing is a prototype currently, lets move to make it more gamified
-       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here</t>
-  </si>
-  <si>
     <t>Balance this thang</t>
   </si>
   <si>
@@ -69,26 +65,6 @@
 ball contacts, blocks, hits ball hitting the ground, success sound, fail sound etc.
 announcer lines to take place of the debug text currently being printed, with several variations for each
 some light music for menus and gameplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
- First step here is to get the AI blockers to move into a better position to defend agains the player
- There are 3 AI blockers at any time and they are in positions 2, 3 and 4 
- I have the RotationManager script tracking each pawns position (RotationManager.aiPositionsArray[2], aiPositionsArray[3] and aiPositionsArray[4] are the AI blockers
-STEP 1: A function that will have the AI blockers move one (or x) square(s) closer to where the player has set the ball
- this function will be called in the RallyManagerV2 script after the player makes their set choice, but before the player decides where they want to attack the ball
-STEP 2: adding on to step 1, if a blocker is &gt;3 squares away from the ball in the y axis, they will move one square towards the ball and one square away from the net
-STEP 3: Some functionality for setting the AI blockers position based on their "matchup" on the other side
- AI blockers will position themselves directly across from their matchup, the matchups are as follows:
-aiPositionsArray[2] matches up with playerPositionsArray[4]
-aiPositionsArray[3] matches up with playerPositionsArray[3]
-aiPositionsArray[4] matches up with playerPositionsArray[2], basically the match ups are who would be standing across the net from each other in the front row
- if one of the match ups is a setter, that player should line up in front of a different front row player, sharing a match up with one of their fellow blockers. So this means when the player setter is in the front row, there will always be 2 ai lined up on one front row playerpawn and 1 ai lined up on the other front row playerpawn
-TDLR
-Step 1: AI blockers move towards the ball to try and block it once the player has made a set
-Step 2: AI blocker that is not close enough to block, steps away from the net and becomes an additional defender
-Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
-</t>
   </si>
   <si>
     <t>Debug this bitch</t>
@@ -162,6 +138,54 @@
       <t xml:space="preserve">need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
+ First step here is to get the AI blockers to move into a better position to defend agains the player
+ There are 3 AI blockers at any time and they are in positions 2, 3 and 4 
+ I have the RotationManager script tracking each pawns position (RotationManager.aiPositionsArray[2], aiPositionsArray[3] and aiPositionsArray[4] are the AI blockers
+STEP 1: A function that will have the AI blockers move one (or x) square(s) closer to where the player has set the ball
+ this function will be called in the RallyManagerV2 script after the player makes their set choice, but before the player decides where they want to attack the ball
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">STEP 2: adding on to step 1, if a blocker is &gt;3 squares away from the ball in the y axis, they will move one square towards the ball and one square away from the net
+STEP 3: Some functionality for setting the AI blockers position based on their "matchup" on the other side
+ AI blockers will position themselves directly across from their matchup, the matchups are as follows:
+aiPositionsArray[2] matches up with playerPositionsArray[4]
+aiPositionsArray[3] matches up with playerPositionsArray[3]
+aiPositionsArray[4] matches up with playerPositionsArray[2], basically the match ups are who would be standing across the net from each other in the front row
+ if one of the match ups is a setter, that player should line up in front of a different front row player, sharing a match up with one of their fellow blockers. So this means when the player setter is in the front row, there will always be 2 ai lined up on one front row playerpawn and 1 ai lined up on the other front row playerpawn
+TDLR
+Step 1: AI blockers move towards the ball to try and block it once the player has made a set
+Step 2: AI blocker that is not close enough to block, steps away from the net and becomes an additional defender
+Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>This thing is a prototype currently, lets move to make it more gamified
+       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here
+       get us to a place where we can generate builds and they'll actually be playable
+       a set up to run multiple scenes so that I can customize the ai behaviour and pawn skill sliders for each differen scene
+       potentially an options menu, allow players to set things like sound volume
+       potentially a credits page that has links to both our portfolio websites
+       any thoughts about art? making this thing look better?</t>
+  </si>
 </sst>
 </file>
 
@@ -184,14 +208,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF92D050"/>
       <name val="Calibri"/>
@@ -529,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -558,62 +582,62 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>14</v>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="345" x14ac:dyDescent="0.25">
@@ -624,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Major update to the features list, added a bunch of polish items and minor features to take this game to the next level
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF39F274-3DCA-4B75-A89C-1B9802356102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCECA55-80D6-433B-9621-BB490ABB2045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Features to be added</t>
   </si>
@@ -49,34 +49,92 @@
   </si>
   <si>
     <t>Balance this thang</t>
+  </si>
+  <si>
+    <t>Add some sounds you idiot</t>
+  </si>
+  <si>
+    <t>Add some basic sound manager functionality into the game
+ball contacts, blocks, hits ball hitting the ground, success sound, fail sound etc.
+announcer lines to take place of the debug text currently being printed, with several variations for each
+some light music for menus and gameplay</t>
+  </si>
+  <si>
+    <t>Debug this bitch</t>
+  </si>
+  <si>
+    <t>Serve Receive Rotation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
+Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
+    </r>
+  </si>
+  <si>
+    <t>This thing is a prototype currently, lets move to make it more gamified
+       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here
+       get us to a place where we can generate builds and they'll actually be playable
+       a set up to run multiple scenes so that I can customize the ai behaviour and pawn skill sliders for each differen scene
+       potentially an options menu, allow players to set things like sound volume
+       potentially a credits page that has links to both our portfolio websites
+       any thoughts about art? making this thing look better?</t>
   </si>
   <si>
     <t>Game is quite unbalanced currently, take another look at each interaction and adjust the numbers so the results make more sense
 Examples: 
 tools more likely when the attacker hitting at only one hand, rather than two.
 Players make more digs when the ball is near them, and less digs when the ball is farther away
-back row players are less likely to score than front row players, but also less likely to get blocked</t>
-  </si>
-  <si>
-    <t>Add some sounds you idiot</t>
-  </si>
-  <si>
-    <t>Add some basic sound manager functionality into the game
-ball contacts, blocks, hits ball hitting the ground, success sound, fail sound etc.
-announcer lines to take place of the debug text currently being printed, with several variations for each
-some light music for menus and gameplay</t>
-  </si>
-  <si>
-    <t>Debug this bitch</t>
-  </si>
-  <si>
-    <t>when the setter makes a dig, have someone else come in and set the ball</t>
-  </si>
-  <si>
-    <t>Setter updates</t>
-  </si>
-  <si>
-    <t>Serve Receive Rotation</t>
+back row players are less likely to score than front row players, but also less likely to get blocked
+balance serve and serve recieve - too many aces and misses for no clear reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
+ First step here is to get the AI blockers to move into a better position to defend agains the player
+ There are 3 AI blockers at any time and they are in positions 2, 3 and 4 
+ I have the RotationManager script tracking each pawns position (RotationManager.aiPositionsArray[2], aiPositionsArray[3] and aiPositionsArray[4] are the AI blockers
+STEP 1: A function that will have the AI blockers move one (or x) square(s) closer to where the player has set the ball
+ this function will be called in the RallyManagerV2 script after the player makes their set choice, but before the player decides where they want to attack the ball
+STEP 2: adding on to step 1, if a blocker is &gt;3 squares away from the ball in the y axis, they will move one square towards the ball and one square away from the net
+STEP 3: Some functionality for setting the AI blockers position based on their "matchup" on the other side
+ AI blockers will position themselves directly across from their matchup, the matchups are as follows:
+aiPositionsArray[2] matches up with playerPositionsArray[4]
+aiPositionsArray[3] matches up with playerPositionsArray[3]
+aiPositionsArray[4] matches up with playerPositionsArray[2], basically the match ups are who would be standing across the net from each other in the front row
+ if one of the match ups is a setter, that player should line up in front of a different front row player, sharing a match up with one of their fellow blockers. So this means when the player setter is in the front row, there will always be 2 ai lined up on one front row playerpawn and 1 ai lined up on the other front row playerpawn
+TDLR
+Step 1: AI blockers move towards the ball to try and block it once the player has made a set
+Step 2: AI blocker that is not close enough to block, steps away from the net and becomes an additional defender
+Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
+</t>
+  </si>
+  <si>
+    <t>Polish / Realization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-&gt; animate the ball properly when the serve or hit goes out of bounds
+(-&gt; animate the player to proper position when serving (off the end line)
+(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
+</t>
   </si>
   <si>
     <r>
@@ -113,20 +171,6 @@
 when calculating the closest pawn, use the updated location and not the indicators location
 stupid ass bug where sometimes after a while of playing, the ball does not get set properly to the servers location (Maybe Fixed) Finally fixed this thing (was moving the digging/passing player towards the ball without releasing their tile)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
-Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
-</t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -135,56 +179,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
+      <t xml:space="preserve">
+(-&gt; fix bug where player can stack their back row players as blockers</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
- First step here is to get the AI blockers to move into a better position to defend agains the player
- There are 3 AI blockers at any time and they are in positions 2, 3 and 4 
- I have the RotationManager script tracking each pawns position (RotationManager.aiPositionsArray[2], aiPositionsArray[3] and aiPositionsArray[4] are the AI blockers
-STEP 1: A function that will have the AI blockers move one (or x) square(s) closer to where the player has set the ball
- this function will be called in the RallyManagerV2 script after the player makes their set choice, but before the player decides where they want to attack the ball
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">STEP 2: adding on to step 1, if a blocker is &gt;3 squares away from the ball in the y axis, they will move one square towards the ball and one square away from the net
-STEP 3: Some functionality for setting the AI blockers position based on their "matchup" on the other side
- AI blockers will position themselves directly across from their matchup, the matchups are as follows:
-aiPositionsArray[2] matches up with playerPositionsArray[4]
-aiPositionsArray[3] matches up with playerPositionsArray[3]
-aiPositionsArray[4] matches up with playerPositionsArray[2], basically the match ups are who would be standing across the net from each other in the front row
- if one of the match ups is a setter, that player should line up in front of a different front row player, sharing a match up with one of their fellow blockers. So this means when the player setter is in the front row, there will always be 2 ai lined up on one front row playerpawn and 1 ai lined up on the other front row playerpawn
-TDLR
-Step 1: AI blockers move towards the ball to try and block it once the player has made a set
-Step 2: AI blocker that is not close enough to block, steps away from the net and becomes an additional defender
-Step 3: AI will line themselves up properly against the players pawns, so that they try to have at least one blocker on each of the players attackers (and so the player can use this to their advantage)
-</t>
-    </r>
-  </si>
-  <si>
-    <t>This thing is a prototype currently, lets move to make it more gamified
-       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here
-       get us to a place where we can generate builds and they'll actually be playable
-       a set up to run multiple scenes so that I can customize the ai behaviour and pawn skill sliders for each differen scene
-       potentially an options menu, allow players to set things like sound volume
-       potentially a credits page that has links to both our portfolio websites
-       any thoughts about art? making this thing look better?</t>
+    <t>AI Attacking</t>
+  </si>
+  <si>
+    <t>Blocking system balance</t>
+  </si>
+  <si>
+    <t>(-&gt; shrink the blockers range
+(-&gt; make it far more likely that an attack made directly at the block will get blocked, and an attack at one hand is likely a tool
+(-&gt; make it so that an attack made with no block is very likely to score
+(-&gt; experiment with blockers being able to move two squares</t>
+  </si>
+  <si>
+    <t>Visual Upgrades</t>
+  </si>
+  <si>
+    <t>(-&gt; running animation for players moving into position
+(-&gt; improved background art and ui button art for the gameplay buttons</t>
+  </si>
+  <si>
+    <t>(-&gt; have the ai check a few different hitting options (line, sharp cross, deep cross, straight down middle, deep middle) and pick from them
+can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
+(-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
+can use AI's hitting percentage and other stats to determine when to change</t>
   </si>
 </sst>
 </file>
@@ -256,19 +278,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,17 +575,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D6" sqref="B6:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="64" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -582,21 +604,21 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -604,209 +626,222 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Fixed a bug where player could have their back row players block
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCECA55-80D6-433B-9621-BB490ABB2045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FA129-102E-48EE-B80A-61F264FF6C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,11 +130,36 @@
     <t>Polish / Realization</t>
   </si>
   <si>
-    <t xml:space="preserve">(-&gt; animate the ball properly when the serve or hit goes out of bounds
+    <t>AI Attacking</t>
+  </si>
+  <si>
+    <t>Blocking system balance</t>
+  </si>
+  <si>
+    <t>(-&gt; shrink the blockers range
+(-&gt; make it far more likely that an attack made directly at the block will get blocked, and an attack at one hand is likely a tool
+(-&gt; make it so that an attack made with no block is very likely to score
+(-&gt; experiment with blockers being able to move two squares</t>
+  </si>
+  <si>
+    <t>Visual Upgrades</t>
+  </si>
+  <si>
+    <t>(-&gt; running animation for players moving into position
+(-&gt; improved background art and ui button art for the gameplay buttons</t>
+  </si>
+  <si>
+    <t>(-&gt; have the ai check a few different hitting options (line, sharp cross, deep cross, straight down middle, deep middle) and pick from them
+can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
+(-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
+can use AI's hitting percentage and other stats to determine when to change</t>
+  </si>
+  <si>
+    <t>(-&gt; animate the ball properly when the serve or hit goes out of bounds
 (-&gt; animate the player to proper position when serving (off the end line)
 (-&gt; have the ball spin/rotate slightly or a lot for different contacts
 (-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
-</t>
+(-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
   </si>
   <si>
     <r>
@@ -180,33 +205,18 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-(-&gt; fix bug where player can stack their back row players as blockers</t>
+</t>
     </r>
-  </si>
-  <si>
-    <t>AI Attacking</t>
-  </si>
-  <si>
-    <t>Blocking system balance</t>
-  </si>
-  <si>
-    <t>(-&gt; shrink the blockers range
-(-&gt; make it far more likely that an attack made directly at the block will get blocked, and an attack at one hand is likely a tool
-(-&gt; make it so that an attack made with no block is very likely to score
-(-&gt; experiment with blockers being able to move two squares</t>
-  </si>
-  <si>
-    <t>Visual Upgrades</t>
-  </si>
-  <si>
-    <t>(-&gt; running animation for players moving into position
-(-&gt; improved background art and ui button art for the gameplay buttons</t>
-  </si>
-  <si>
-    <t>(-&gt; have the ai check a few different hitting options (line, sharp cross, deep cross, straight down middle, deep middle) and pick from them
-can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
-(-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
-can use AI's hitting percentage and other stats to determine when to change</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-&gt; fix bug where player can stack their back row players as blockers</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -575,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +647,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
@@ -648,18 +658,18 @@
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -675,24 +685,24 @@
     </row>
     <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Out of bounds serves and attacks should now animate properly outside the court
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FA129-102E-48EE-B80A-61F264FF6C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DABC5D0-C73D-45FE-AECD-207A5BCC95B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,13 +153,6 @@
 can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
 (-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
 can use AI's hitting percentage and other stats to determine when to change</t>
-  </si>
-  <si>
-    <t>(-&gt; animate the ball properly when the serve or hit goes out of bounds
-(-&gt; animate the player to proper position when serving (off the end line)
-(-&gt; have the ball spin/rotate slightly or a lot for different contacts
-(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
-(-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
   </si>
   <si>
     <r>
@@ -216,6 +209,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>(-&gt; fix bug where player can stack their back row players as blockers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-&gt; animate the ball properly when the serve or hit goes out of bounds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(-&gt; animate the player to proper position when serving (off the end line)
+(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
+(-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
     </r>
   </si>
 </sst>
@@ -585,13 +604,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="64" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
@@ -647,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
@@ -658,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Set the servers to start with the ball on the endline of the court, instead of inside the court
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DABC5D0-C73D-45FE-AECD-207A5BCC95B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEC2C69-E776-4A51-92FB-213670FD701A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,8 +231,28 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-(-&gt; animate the player to proper position when serving (off the end line)
-(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(-&gt; animate the player to proper position when serving (off the end line)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-&gt; have the ball spin/rotate slightly or a lot for different contacts
 (-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
 (-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
     </r>

</xml_diff>

<commit_message>
Now tools actually leave the court boundaries, and randomly move to same side or opposite side of court
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEC2C69-E776-4A51-92FB-213670FD701A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750E9E94-967F-46BE-9463-4002FB0CF3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,6 +242,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">(-&gt; animate the player to proper position when serving (off the end line)
+(-&gt; animated the tool to go out of bounds
 </t>
     </r>
     <r>
@@ -624,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Ball now travels in a line towards its destination before contacting the block, should now look proper with tools and blocks commented out some debug
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750E9E94-967F-46BE-9463-4002FB0CF3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB6CCB8-66C3-4D40-A011-70A6F91140A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,8 +253,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(-&gt; have the ball spin/rotate slightly or a lot for different contacts
-(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
+      <t xml:space="preserve">(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
 (-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
     </r>
   </si>
@@ -626,17 +636,17 @@
   <dimension ref="B3:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -658,7 +668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -669,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -680,7 +690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -691,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -702,7 +712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -713,7 +723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -724,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -735,7 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -746,7 +756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="345" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
@@ -757,142 +767,142 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
AI attackers now analyze their hitting options before choosing an attack location, will pick the location with the least opponent blockers
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB6CCB8-66C3-4D40-A011-70A6F91140A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF847E1-B4A7-43A9-B697-5345AD117222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,12 +149,6 @@
 (-&gt; improved background art and ui button art for the gameplay buttons</t>
   </si>
   <si>
-    <t>(-&gt; have the ai check a few different hitting options (line, sharp cross, deep cross, straight down middle, deep middle) and pick from them
-can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
-(-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
-can use AI's hitting percentage and other stats to determine when to change</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -241,8 +235,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(-&gt; animate the player to proper position when serving (off the end line)
+      <t>(-&gt; animate the player to proper position when serving (off the end line)
 (-&gt; animated the tool to go out of bounds
+(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
+(-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(-&gt; have the ai check a few different hitting options (line, sharp cross, deep cross, straight down middle, deep middle) and pick from them
+can use the raycast system to check each shot for which has the least blockers, or pick a tool opportunity
 </t>
     </r>
     <r>
@@ -253,7 +263,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(-&gt; have the ball spin/rotate slightly or a lot for different contacts
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -264,8 +274,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(-&gt; animate the tools properly, have the ball move towards the blocker it contacted then spin off to tool location
-(-&gt; animate the blocks properly, have the ball move towards the blocker it contacted then go back into players court</t>
+      <t>(-&gt; added a random moving of AI attackers as a start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
+can use AI's hitting percentage and other stats to determine when to change</t>
     </r>
   </si>
 </sst>
@@ -635,18 +656,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -668,7 +689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -679,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -690,7 +711,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -698,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -709,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -720,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -734,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -745,7 +766,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -756,7 +777,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
@@ -767,142 +788,142 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Updated feature list, going to do an ai coach solution for the ai attacking positions
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF847E1-B4A7-43A9-B697-5345AD117222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15EAE6A-550E-4742-824F-F241754A3C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,8 @@
       </rPr>
       <t xml:space="preserve">
 (-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
-can use AI's hitting percentage and other stats to determine when to change</t>
+can use AI's hitting percentage and other stats to determine when to change
+(-&gt; can make functions in the ai coach script to return y and x locations for the ai attackers based on situation, that way can be precise about where they will set up, and so its not completely random</t>
     </r>
   </si>
 </sst>
@@ -733,7 +734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Added and clipped some sprite sheets for both players, created a new scene to work with and test the animations
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15EAE6A-550E-4742-824F-F241754A3C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A0E8F-F0D7-482B-AAA2-15AE637D9E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Features to be added</t>
   </si>
@@ -145,10 +145,6 @@
     <t>Visual Upgrades</t>
   </si>
   <si>
-    <t>(-&gt; running animation for players moving into position
-(-&gt; improved background art and ui button art for the gameplay buttons</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -285,10 +281,31 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 (-&gt; have the AI coach determine different offensive attacking linups for the AI to set up in
 can use AI's hitting percentage and other stats to determine when to change
 (-&gt; can make functions in the ai coach script to return y and x locations for the ai attackers based on situation, that way can be precise about where they will set up, and so its not completely random</t>
     </r>
+  </si>
+  <si>
+    <t>Player Animations</t>
+  </si>
+  <si>
+    <t>(-&gt; add animations for both player and AI
+(-&gt; hook up animations to each specific phase</t>
+  </si>
+  <si>
+    <t>(-&gt; improved background art and ui button art for the gameplay buttons</t>
   </si>
 </sst>
 </file>
@@ -657,18 +674,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -690,7 +707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -701,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -712,7 +729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -720,10 +737,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -731,10 +748,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -742,10 +759,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -756,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -767,7 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -775,156 +792,162 @@
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Fixed some minor bugs with comp spike animation and rotation 4 for comp player
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A0E8F-F0D7-482B-AAA2-15AE637D9E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806EA3A3-BBFC-4006-AE85-C108BAD8641D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -301,11 +301,31 @@
     <t>Player Animations</t>
   </si>
   <si>
-    <t>(-&gt; add animations for both player and AI
-(-&gt; hook up animations to each specific phase</t>
-  </si>
-  <si>
     <t>(-&gt; improved background art and ui button art for the gameplay buttons</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(-&gt; add animations for both player and AI
+(-&gt; hook up animations to each specific phase
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -674,18 +694,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -707,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -718,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -729,7 +749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -740,7 +760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -751,7 +771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -762,7 +782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -773,7 +793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -784,7 +804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -792,10 +812,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
@@ -803,10 +823,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
@@ -817,137 +837,137 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Added animations for player movment in 8 directions, set up triggers to pick the correct movement direction
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806EA3A3-BBFC-4006-AE85-C108BAD8641D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202CF89E-AE88-4C96-A256-42051AFE9A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,28 +304,9 @@
     <t>(-&gt; improved background art and ui button art for the gameplay buttons</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(-&gt; add animations for both player and AI
+    <t>(-&gt; add animations for both player and AI
 (-&gt; hook up animations to each specific phase
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
-    </r>
+(-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
   </si>
 </sst>
 </file>
@@ -384,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,6 +391,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,17 +679,17 @@
   <dimension ref="B3:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -727,7 +711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -738,7 +722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -749,7 +733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -760,7 +744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -771,7 +755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -782,7 +766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -793,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -804,7 +788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -815,18 +799,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
@@ -837,137 +821,137 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Did some balance work increased importance of distance from the ball for digging and serve recieve Increased blockers reaction distance to 2 tiles, keeping it at 1 tile for 3 passes altered service range to include a small chance to serve 3 tiles away added specific values for when the attacker is attacking against a 1 hand block, more likely to tool updated the prefab to shrink the blockers influence range some other minor balancing updates
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202CF89E-AE88-4C96-A256-42051AFE9A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A11CD2D-4BDF-4368-833C-031F24E91C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,14 +97,6 @@
        potentially an options menu, allow players to set things like sound volume
        potentially a credits page that has links to both our portfolio websites
        any thoughts about art? making this thing look better?</t>
-  </si>
-  <si>
-    <t>Game is quite unbalanced currently, take another look at each interaction and adjust the numbers so the results make more sense
-Examples: 
-tools more likely when the attacker hitting at only one hand, rather than two.
-Players make more digs when the ball is near them, and less digs when the ball is farther away
-back row players are less likely to score than front row players, but also less likely to get blocked
-balance serve and serve recieve - too many aces and misses for no clear reason</t>
   </si>
   <si>
     <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
@@ -307,6 +299,46 @@
     <t>(-&gt; add animations for both player and AI
 (-&gt; hook up animations to each specific phase
 (-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Game is quite unbalanced currently, take another look at each interaction and adjust the numbers so the results make more sense
+Examples: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tools more likely when the attacker hitting at only one hand, rather than two.
+Players make more digs when the ball is near them, and less digs when the ball is farther away</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+back row players are less likely to score than front row players, but also less likely to get blocked
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>balance serve and serve recieve - too many aces and misses for no clear reason</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -678,18 +710,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="B14:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -711,7 +743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -722,7 +754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -730,10 +762,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -741,32 +773,32 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -777,40 +809,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="10" t="s">
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
@@ -818,140 +850,140 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Made it so that back row players are less likely to contact the block with their attacks, and also more likely to get dug by defenders
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\VolleyballSimGameRepository\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A11CD2D-4BDF-4368-833C-031F24E91C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7541F995-2186-4E96-AEA5-F21FCEF0645A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,30 +64,6 @@
   </si>
   <si>
     <t>Serve Receive Rotation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
-Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">need some sort of prompt to the player that they attempted to place their piece out of rotation. </t>
-    </r>
   </si>
   <si>
     <t>This thing is a prototype currently, lets move to make it more gamified
@@ -301,6 +277,11 @@
 (-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
   </si>
   <si>
+    <t xml:space="preserve">Make it so that whenever the player is changing around their serve receive positions, they are unable to place their players out of rotation.
+Likely need a function to check whether or not an attempted placement is valid, and then not allowing the player to move beyond that space, similar to the limited movement during reaction phases
+</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Game is quite unbalanced currently, take another look at each interaction and adjust the numbers so the results make more sense
 Examples: 
@@ -326,7 +307,27 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-back row players are less likely to score than front row players, but also less likely to get blocked
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>back row players are less likely to score than front row players, but also less likely to get blocked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -710,18 +711,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="152" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -740,10 +741,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -754,7 +755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -765,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -773,76 +774,76 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="144" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="331.2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
@@ -850,140 +851,140 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>

<commit_message>
Added a ton of announcer lines, hooked them up to trigger during the rally in game and a few in the menus HILARIOUS
</commit_message>
<xml_diff>
--- a/Documentation/Features List.xlsx
+++ b/Documentation/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Documents\Unity Projects\Volleyball Sim Repository\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7541F995-2186-4E96-AEA5-F21FCEF0645A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69526A93-11E4-473B-8D4B-0D6D51CB8C4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Features to be added</t>
   </si>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>Serve Receive Rotation</t>
-  </si>
-  <si>
-    <t>This thing is a prototype currently, lets move to make it more gamified
-       add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here
-       get us to a place where we can generate builds and they'll actually be playable
-       a set up to run multiple scenes so that I can customize the ai behaviour and pawn skill sliders for each differen scene
-       potentially an options menu, allow players to set things like sound volume
-       potentially a credits page that has links to both our portfolio websites
-       any thoughts about art? making this thing look better?</t>
   </si>
   <si>
     <t xml:space="preserve"> Idea here is to get the AI to start actually doing things to defend against the player, start making this feel like a game
@@ -110,9 +101,6 @@
 (-&gt; experiment with blockers being able to move two squares</t>
   </si>
   <si>
-    <t>Visual Upgrades</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -269,9 +257,6 @@
     <t>Player Animations</t>
   </si>
   <si>
-    <t>(-&gt; improved background art and ui button art for the gameplay buttons</t>
-  </si>
-  <si>
     <t>(-&gt; add animations for both player and AI
 (-&gt; hook up animations to each specific phase
 (-&gt; add specific directional dive and movement animations that trigger depending on the direction the player is moving</t>
@@ -339,6 +324,78 @@
         <scheme val="minor"/>
       </rPr>
       <t>balance serve and serve recieve - too many aces and misses for no clear reason</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This thing is a prototype currently, lets move to make it more gamified
+       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add a menu system with buttons to start a game, an option to quit to menu from game, an option to quit the game entirely, etc. Add whatever makes sense here</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get us to a place where we can generate builds and they'll actually be playable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a set up to run multiple scenes so that I can customize the ai behaviour and pawn skill sliders for each differen scene</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       potentially an options menu, allow players to set things like sound volume
+       potentially a credits page that has links to both our portfolio websites
+       pause menu that has the option to include game statistics (I am tracking these already) and to quit the game
+       any thoughts about art? making this thing look better? any other stuff we need to put this thing out there?</t>
     </r>
   </si>
 </sst>
@@ -711,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -733,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -741,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
@@ -763,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="105" x14ac:dyDescent="0.25">
@@ -774,29 +831,29 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
@@ -807,40 +864,34 @@
         <v>4</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="345" x14ac:dyDescent="0.25">
@@ -851,7 +902,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>